<commit_message>
Revert "Re use scenario 1"
</commit_message>
<xml_diff>
--- a/Westwood_TUFLOW_modelling_log.xlsx
+++ b/Westwood_TUFLOW_modelling_log.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="132">
   <si>
     <t>Project Name:</t>
   </si>
@@ -417,18 +417,6 @@
   </si>
   <si>
     <t>changed inflow location of westwood creek</t>
-  </si>
-  <si>
-    <t>ReUse Scenario 1</t>
-  </si>
-  <si>
-    <t>fdgdfg</t>
-  </si>
-  <si>
-    <t>SM</t>
-  </si>
-  <si>
-    <t>013</t>
   </si>
 </sst>
 </file>
@@ -1020,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34:I36"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1456,164 +1444,6 @@
       </c>
       <c r="I21" s="11" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24"/>
-      <c r="C24" t="s">
-        <v>132</v>
-      </c>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
-      <c r="J24"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25"/>
-      <c r="C25" t="s">
-        <v>133</v>
-      </c>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25"/>
-      <c r="I25"/>
-      <c r="J25"/>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26"/>
-      <c r="C26" t="s">
-        <v>134</v>
-      </c>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
-      <c r="G26"/>
-      <c r="H26"/>
-      <c r="I26"/>
-      <c r="J26"/>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27"/>
-      <c r="F27"/>
-      <c r="G27"/>
-      <c r="H27"/>
-      <c r="I27"/>
-      <c r="J27"/>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28"/>
-      <c r="C28" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28"/>
-      <c r="J28"/>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
-      <c r="J29"/>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30"/>
-      <c r="I30"/>
-      <c r="J30"/>
-    </row>
-    <row r="31" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31"/>
-      <c r="J31"/>
-    </row>
-    <row r="32" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J32" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B33" s="13">
-        <v>42612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>